<commit_message>
Refactor code to separate out model training, text pre processing, and running the prediction model.
</commit_message>
<xml_diff>
--- a/Data/Test_Proposal_Data_1.xlsx
+++ b/Data/Test_Proposal_Data_1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhans\PycharmProjects\Agenda Mapping ML\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhans\PycharmProjects\Agenda_Mapping_ML\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587710C9-0F1B-4ABF-95F1-0F3EE75E7F20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AF7CA26-2B4F-4979-8204-D8CC99E1F3E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4776" yWindow="2556" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,14 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>proposal_text</t>
   </si>
   <si>
-    <t>issue_code</t>
-  </si>
-  <si>
     <t>Elect Sarah Hansen</t>
   </si>
   <si>
@@ -109,6 +106,12 @@
   </si>
   <si>
     <t>Shareholder Proposal No. 1</t>
+  </si>
+  <si>
+    <t>Appointment of Samwise as auditor for fiscal year 2024</t>
+  </si>
+  <si>
+    <t>Director election of silly sally</t>
   </si>
 </sst>
 </file>
@@ -426,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:A29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -437,142 +440,149 @@
     <col min="1" max="1" width="34.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>